<commit_message>
Mete iteration - update on timelines for diff hangers
</commit_message>
<xml_diff>
--- a/Timelines/powertrain projects.xlsx
+++ b/Timelines/powertrain projects.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Retro\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/metehergul/Documents/fbr23 projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700CB308-487D-4588-ABCB-92DBAC840705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C77AFAB-4DFC-A943-BB46-344400FAE3A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="40960" windowHeight="25600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exhaust" sheetId="5" r:id="rId1"/>
-    <sheet name="sprocket" sheetId="10" r:id="rId2"/>
-    <sheet name="Intake" sheetId="1" r:id="rId3"/>
-    <sheet name="diff hangers" sheetId="4" r:id="rId4"/>
+    <sheet name="Intake" sheetId="1" r:id="rId2"/>
+    <sheet name="diff hangers" sheetId="4" r:id="rId3"/>
+    <sheet name="sprocket" sheetId="10" r:id="rId4"/>
     <sheet name="Rear rad" sheetId="6" r:id="rId5"/>
     <sheet name="Chassis bar (incomplete)" sheetId="7" r:id="rId6"/>
     <sheet name="Design Goals" sheetId="2" r:id="rId7"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="126">
   <si>
     <t>Task 1:</t>
   </si>
@@ -242,21 +242,9 @@
     <t>intertwined with chassis design</t>
   </si>
   <si>
-    <t>NC; Tasin &amp; Mete</t>
-  </si>
-  <si>
     <t>1, 3, 6</t>
   </si>
   <si>
-    <t>Chassis</t>
-  </si>
-  <si>
-    <t>Cutting</t>
-  </si>
-  <si>
-    <t>solid amount of fea preferred, need in time for dyno</t>
-  </si>
-  <si>
     <t>Sprocket and Carrier</t>
   </si>
   <si>
@@ -275,12 +263,6 @@
     <t>attention to prevent repeat of fbr22 intake incident. not very prototypable, pay attention to not throw money &amp; time out the window</t>
   </si>
   <si>
-    <t>(First two design iterations are fresher playground, the other two are real)</t>
-  </si>
-  <si>
-    <t>Design iteration 4 done</t>
-  </si>
-  <si>
     <t>1-2 weeks</t>
   </si>
   <si>
@@ -311,9 +293,6 @@
     <t>noise test, quick drive</t>
   </si>
   <si>
-    <t>20 + 05h</t>
-  </si>
-  <si>
     <t>1 week</t>
   </si>
   <si>
@@ -411,6 +390,27 @@
   </si>
   <si>
     <t xml:space="preserve">£40 - for 700g filament option. I suspect </t>
+  </si>
+  <si>
+    <t>*Prompt solution, may be re-done as required</t>
+  </si>
+  <si>
+    <t>Mete</t>
+  </si>
+  <si>
+    <t>Tasin,  interested fresher(s)</t>
+  </si>
+  <si>
+    <t>(First design iteration is fresher playground, the other two are real)</t>
+  </si>
+  <si>
+    <t>Postponed due to diff hanger failure</t>
+  </si>
+  <si>
+    <t>I accidentally deleted your meeting slot here Aidan, it's what was originally for sprocket and carrier</t>
+  </si>
+  <si>
+    <t>Design iteration 3</t>
   </si>
 </sst>
 </file>
@@ -418,9 +418,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="6" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
-    <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
-    <numFmt numFmtId="165" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="166" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -505,19 +505,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="6" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -897,14 +898,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>266139</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>301884</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>35745</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>17477</xdr:rowOff>
     </xdr:to>
@@ -929,8 +930,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="896470" y="0"/>
-          <a:ext cx="9490708" cy="4934058"/>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9211204" cy="5208165"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -941,16 +942,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>224117</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>105055</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>454034</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>75360</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>225155</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -973,8 +974,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="854448" y="5021636"/>
-          <a:ext cx="9684880" cy="5068981"/>
+          <a:off x="0" y="5143500"/>
+          <a:ext cx="9369155" cy="5295900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -986,15 +987,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>161085</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>56029</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>94265</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>563511</xdr:colOff>
       <xdr:row>83</xdr:row>
-      <xdr:rowOff>181831</xdr:rowOff>
+      <xdr:rowOff>125802</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1017,8 +1018,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="161085" y="10071286"/>
-          <a:ext cx="10018474" cy="5224479"/>
+          <a:off x="0" y="10872877"/>
+          <a:ext cx="9729077" cy="5661085"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1030,15 +1031,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>77040</xdr:colOff>
-      <xdr:row>84</xdr:row>
-      <xdr:rowOff>32634</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>174948</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>85643</xdr:colOff>
+      <xdr:colOff>8603</xdr:colOff>
       <xdr:row>111</xdr:row>
-      <xdr:rowOff>175852</xdr:rowOff>
+      <xdr:rowOff>136071</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1061,8 +1062,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="77040" y="15328663"/>
-          <a:ext cx="10093897" cy="5059799"/>
+          <a:off x="0" y="16309132"/>
+          <a:ext cx="9650236" cy="5403980"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1073,16 +1074,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>161085</xdr:colOff>
-      <xdr:row>111</xdr:row>
-      <xdr:rowOff>144837</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>162374</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>1289</xdr:colOff>
       <xdr:row>139</xdr:row>
-      <xdr:rowOff>143891</xdr:rowOff>
+      <xdr:rowOff>176389</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1105,8 +1106,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="791416" y="20357447"/>
-          <a:ext cx="10086583" cy="5097731"/>
+          <a:off x="0" y="21731112"/>
+          <a:ext cx="9879067" cy="5415138"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1117,16 +1118,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>287151</xdr:colOff>
-      <xdr:row>143</xdr:row>
-      <xdr:rowOff>74800</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>287151</xdr:colOff>
-      <xdr:row>172</xdr:row>
-      <xdr:rowOff>12696</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>168</xdr:row>
+      <xdr:rowOff>119991</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1149,8 +1150,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="917482" y="26114469"/>
-          <a:ext cx="10085294" cy="5218668"/>
+          <a:off x="1" y="26670000"/>
+          <a:ext cx="9652000" cy="5453991"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1428,21 +1429,21 @@
   <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.46484375" customWidth="1"/>
+    <col min="1" max="1" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1450,7 +1451,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -1458,7 +1459,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1467,7 +1468,7 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1475,7 +1476,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1484,13 +1485,13 @@
       </c>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>64</v>
       </c>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1499,7 +1500,7 @@
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1508,7 +1509,7 @@
       </c>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1517,7 +1518,7 @@
       </c>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1525,10 +1526,10 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1537,7 +1538,7 @@
       </c>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1546,7 +1547,7 @@
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1557,7 +1558,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -1565,7 +1566,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1573,7 +1574,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -1584,20 +1585,20 @@
         <v>500</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>50</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="6"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -1605,7 +1606,7 @@
         <v>44850</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -1613,10 +1614,10 @@
         <v>44851</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -1624,7 +1625,7 @@
         <v>44858</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -1632,10 +1633,10 @@
         <v>44864</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -1643,10 +1644,10 @@
         <v>44867</v>
       </c>
       <c r="C25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1654,7 +1655,7 @@
         <v>44874</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -1662,7 +1663,7 @@
         <v>44888</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -1671,58 +1672,58 @@
       </c>
       <c r="C28" s="6"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" s="3"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" s="3"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" s="3"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B37" s="3"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B38" s="3"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B39" s="3"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B41" s="3"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B42" s="3"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B43" s="3"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B44" s="3"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B45" s="3"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B46" s="3"/>
     </row>
   </sheetData>
@@ -1767,33 +1768,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71F63D42-6AB1-3F4D-96FB-66922EEFB734}">
-  <dimension ref="A1:C47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42" customWidth="1"/>
+    <col min="1" max="1" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -1801,7 +1802,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1810,36 +1811,42 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="7">
         <v>1</v>
       </c>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1848,16 +1855,16 @@
       </c>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="3">
-        <v>44943</v>
+        <v>44972</v>
       </c>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1865,196 +1872,189 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>22</v>
       </c>
       <c r="B13" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
       <c r="B14" t="s">
         <v>25</v>
       </c>
-      <c r="C14" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="4">
-        <v>80</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+        <v>150</v>
+      </c>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>50</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C18" s="6"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>67</v>
       </c>
       <c r="B21" s="3">
-        <v>44865</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+        <v>44858</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>37</v>
       </c>
       <c r="B22" s="3">
-        <v>44869</v>
+        <v>44860</v>
       </c>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B23" s="3">
-        <v>44884</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+        <v>44872</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>38</v>
       </c>
       <c r="B24" s="3">
-        <v>44885</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+        <v>44876</v>
+      </c>
+      <c r="C24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>33</v>
       </c>
       <c r="B25" s="3">
         <v>44895</v>
       </c>
-      <c r="C25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>34</v>
       </c>
       <c r="B26" s="3">
-        <v>44936</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+        <v>44949</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>39</v>
       </c>
       <c r="B27" s="3">
-        <v>44943</v>
+        <v>44972</v>
       </c>
       <c r="C27" s="6"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B28" s="3"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B29" s="3"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" s="3"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" s="3"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" s="3"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B37" s="3"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B38" s="3"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B39" s="3"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B41" s="3"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B42" s="3"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B43" s="3"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B44" s="3"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B45" s="3"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B46" s="3"/>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B47" s="3"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="B6">
+  <conditionalFormatting sqref="B6:B7">
     <cfRule type="cellIs" dxfId="34" priority="5" operator="equal">
       <formula>3</formula>
     </cfRule>
@@ -2095,33 +2095,36 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68AAC58C-EBDA-3946-A752-4A750B3F87FB}">
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -2129,24 +2132,24 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>2</v>
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -2155,233 +2158,210 @@
       </c>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>63</v>
-      </c>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="3">
-        <v>44895</v>
+        <v>44874</v>
       </c>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="3">
-        <v>44972</v>
+        <v>44895</v>
       </c>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
       <c r="B11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="4">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="C17" s="6"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>50</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="C18" s="6"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="B21" s="3">
-        <v>44858</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+        <v>44862</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>37</v>
       </c>
       <c r="B22" s="3">
-        <v>44860</v>
-      </c>
-      <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+        <v>44864</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>75</v>
-      </c>
-      <c r="B23" s="3">
-        <v>44872</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+        <v>125</v>
+      </c>
+      <c r="B23" s="12">
+        <v>44874</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B24" s="3">
-        <v>44876</v>
-      </c>
-      <c r="C24" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+        <v>44880</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B25" s="3">
         <v>44895</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" s="3">
-        <v>44949</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" s="3">
-        <v>44972</v>
-      </c>
-      <c r="C27" s="6"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C25" s="6"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B28" s="3"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" s="3"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" s="3"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" s="3"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B37" s="3"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B38" s="3"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B39" s="3"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B41" s="3"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B42" s="3"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B43" s="3"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B44" s="3"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B45" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B6:B7">
+  <conditionalFormatting sqref="B6">
     <cfRule type="cellIs" dxfId="27" priority="5" operator="equal">
       <formula>3</formula>
     </cfRule>
@@ -2422,33 +2402,33 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68AAC58C-EBDA-3946-A752-4A750B3F87FB}">
-  <dimension ref="A1:C45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71F63D42-6AB1-3F4D-96FB-66922EEFB734}">
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.46484375" customWidth="1"/>
+    <col min="1" max="1" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -2456,45 +2436,47 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="8">
         <v>2</v>
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="8">
         <v>1</v>
       </c>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>120</v>
       </c>
       <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E8" s="1"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2502,8 +2484,10 @@
         <v>44927</v>
       </c>
       <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F9" s="3"/>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2511,19 +2495,21 @@
         <v>44995</v>
       </c>
       <c r="C10" s="5"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F10" s="3"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -2531,35 +2517,37 @@
         <v>2</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+        <v>88</v>
+      </c>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -2567,7 +2555,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -2575,31 +2563,38 @@
         <v>80</v>
       </c>
       <c r="C17" s="6"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F17" s="4"/>
+      <c r="G17" s="6"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>50</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>68</v>
+        <v>123</v>
       </c>
       <c r="C18" s="6"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F18" s="4"/>
+      <c r="G18" s="6"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="5"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E20" s="1"/>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>35</v>
       </c>
       <c r="B21" s="3">
         <v>44895</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -2607,16 +2602,19 @@
         <v>44899</v>
       </c>
       <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F22" s="3"/>
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>36</v>
       </c>
       <c r="B23" s="3">
         <v>44913</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -2624,87 +2622,86 @@
         <v>44918</v>
       </c>
       <c r="C24" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+        <v>84</v>
+      </c>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
       <c r="B25" s="3">
-        <v>44927</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+        <v>44971</v>
+      </c>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B26" s="3">
-        <v>44971</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" s="3">
         <v>44995</v>
       </c>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C27" s="6"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B28" s="3"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B29" s="3"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F27" s="3"/>
+      <c r="G27" s="6"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" s="3"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" s="3"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" s="3"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B37" s="3"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B38" s="3"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B39" s="3"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B41" s="3"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B42" s="3"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B43" s="3"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B44" s="3"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B45" s="3"/>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B46" s="3"/>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B47" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B6">
@@ -2755,26 +2752,26 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.46484375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -2782,7 +2779,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2791,15 +2788,15 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -2808,21 +2805,21 @@
       </c>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2830,10 +2827,10 @@
         <v>44883</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2842,7 +2839,7 @@
       </c>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -2850,7 +2847,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -2859,7 +2856,7 @@
       </c>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -2868,7 +2865,7 @@
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2876,26 +2873,26 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -2903,25 +2900,25 @@
         <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>50</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C18" s="6"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -2929,7 +2926,7 @@
         <v>44859</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -2938,15 +2935,15 @@
       </c>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B23" s="3">
         <v>44875</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -2954,10 +2951,10 @@
         <v>44876</v>
       </c>
       <c r="C24" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -2965,7 +2962,7 @@
         <v>44895</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -2973,7 +2970,7 @@
         <v>44897</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -2982,58 +2979,58 @@
       </c>
       <c r="C27" s="6"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B28" s="3"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" s="3"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" s="3"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" s="3"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B37" s="3"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B38" s="3"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B39" s="3"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B41" s="3"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B42" s="3"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B43" s="3"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B44" s="3"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B45" s="3"/>
     </row>
   </sheetData>
@@ -3085,13 +3082,13 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.46484375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3099,7 +3096,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -3107,7 +3104,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -3115,12 +3112,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -3128,7 +3125,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -3136,7 +3133,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -3147,7 +3144,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -3155,7 +3152,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -3166,12 +3163,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C10" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -3182,7 +3179,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -3193,7 +3190,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -3204,7 +3201,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -3212,7 +3209,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -3223,7 +3220,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -3234,7 +3231,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -3242,7 +3239,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -3253,7 +3250,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -3261,7 +3258,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -3272,7 +3269,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -3281,7 +3278,7 @@
       </c>
       <c r="C21" s="6"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
@@ -3289,7 +3286,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -3297,7 +3294,7 @@
         <v>44865</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -3308,7 +3305,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -3316,7 +3313,7 @@
         <v>44884</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -3324,7 +3321,7 @@
         <v>44898</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -3335,7 +3332,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -3343,7 +3340,7 @@
         <v>44954</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -3351,7 +3348,7 @@
         <v>44961</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -3359,7 +3356,7 @@
         <v>44982</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -3370,58 +3367,58 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" s="3"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" s="3"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" s="3"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B37" s="3"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B38" s="3"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B39" s="3"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B41" s="3"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B42" s="3"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B43" s="3"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B44" s="3"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B45" s="3"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B46" s="3"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B47" s="3"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B48" s="3"/>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B49" s="3"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B50" s="3"/>
     </row>
   </sheetData>
@@ -3471,7 +3468,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3482,114 +3479,114 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BE59ABF-F952-490F-B319-5676379536F1}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="159" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>106</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+      <c r="B7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>112</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B8" s="10" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B5" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="C5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B7" t="s">
-        <v>115</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="D7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>119</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>118</v>
       </c>
       <c r="C8" s="11">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C10" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -3609,11 +3606,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="136" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="J171" sqref="J171:K171"/>
+    <sheetView topLeftCell="C105" zoomScale="136" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="R166" sqref="R166"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Minor updates to existing timelines, checked new Diff hanger timeline - Tasin Iteration
</commit_message>
<xml_diff>
--- a/Timelines/powertrain projects.xlsx
+++ b/Timelines/powertrain projects.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/metehergul/Documents/fbr23 projects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Retro\OneDrive\Documents\FBR work\Powertrain Repo\Powertrain-Projects-FBR23\Timelines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C77AFAB-4DFC-A943-BB46-344400FAE3A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D2234B2-957D-47B2-9500-61BF88F86548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="40960" windowHeight="25600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exhaust" sheetId="5" r:id="rId1"/>
-    <sheet name="Intake" sheetId="1" r:id="rId2"/>
-    <sheet name="diff hangers" sheetId="4" r:id="rId3"/>
-    <sheet name="sprocket" sheetId="10" r:id="rId4"/>
-    <sheet name="Rear rad" sheetId="6" r:id="rId5"/>
-    <sheet name="Chassis bar (incomplete)" sheetId="7" r:id="rId6"/>
-    <sheet name="Design Goals" sheetId="2" r:id="rId7"/>
-    <sheet name="Sheet1" sheetId="11" r:id="rId8"/>
-    <sheet name="Major Deadlines" sheetId="3" r:id="rId9"/>
+    <sheet name="Gear position" sheetId="12" r:id="rId2"/>
+    <sheet name="Intake" sheetId="1" r:id="rId3"/>
+    <sheet name="diff hangers" sheetId="4" r:id="rId4"/>
+    <sheet name="sprocket" sheetId="10" r:id="rId5"/>
+    <sheet name="Rear rad" sheetId="6" r:id="rId6"/>
+    <sheet name="Chassis bar (incomplete)" sheetId="7" r:id="rId7"/>
+    <sheet name="Design Goals" sheetId="2" r:id="rId8"/>
+    <sheet name="Estimation of costs" sheetId="11" r:id="rId9"/>
+    <sheet name="Major Deadlines" sheetId="3" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="144">
   <si>
     <t>Task 1:</t>
   </si>
@@ -290,9 +291,6 @@
     <t>TD</t>
   </si>
   <si>
-    <t>noise test, quick drive</t>
-  </si>
-  <si>
     <t>1 week</t>
   </si>
   <si>
@@ -302,18 +300,6 @@
     <t>1 fresher prototype</t>
   </si>
   <si>
-    <t>?fresher</t>
-  </si>
-  <si>
-    <t>?can trixckle into xmas</t>
-  </si>
-  <si>
-    <t>?if we need new parts lead time will extend</t>
-  </si>
-  <si>
-    <t>?if we need new parts lead time will extend £80</t>
-  </si>
-  <si>
     <t>?TD</t>
   </si>
   <si>
@@ -407,10 +393,79 @@
     <t>Postponed due to diff hanger failure</t>
   </si>
   <si>
-    <t>I accidentally deleted your meeting slot here Aidan, it's what was originally for sprocket and carrier</t>
-  </si>
-  <si>
     <t>Design iteration 3</t>
+  </si>
+  <si>
+    <t>1 ideally for primaries, up to 2 for the tertiaries (different muffler positions)</t>
+  </si>
+  <si>
+    <t>TD (done)</t>
+  </si>
+  <si>
+    <t>Driving done - with current muffler arrangement, new tertiaries need manufacturing</t>
+  </si>
+  <si>
+    <t>Noise test, quick drive (after muffler configurations manufactured)</t>
+  </si>
+  <si>
+    <t>Parts will be necessary - no known psonsorship form Siliconhoses</t>
+  </si>
+  <si>
+    <t>Estimation of timeline for Gear position sensor from Arnav - based on plausibility</t>
+  </si>
+  <si>
+    <t>TD - meeting slot for Diff hangers</t>
+  </si>
+  <si>
+    <t>Design discussions</t>
+  </si>
+  <si>
+    <t>3. Dirtbikesuk</t>
+  </si>
+  <si>
+    <t>4. TE Connectivity</t>
+  </si>
+  <si>
+    <t>Chassis bar</t>
+  </si>
+  <si>
+    <t>New parts are required - can be prototyped with current set of tubes</t>
+  </si>
+  <si>
+    <t>Can or fluids iterations can trickle into Xmas</t>
+  </si>
+  <si>
+    <t>CURRENT UPDATE REQUIRED</t>
+  </si>
+  <si>
+    <t>Contacted</t>
+  </si>
+  <si>
+    <t>5. Filaments for 3D printing</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>6. Silicon Hoses</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>N/Y</t>
+  </si>
+  <si>
+    <t>7. Tube Bender</t>
+  </si>
+  <si>
+    <t>Dependent on Chassis + If Lister tube quote is too high, could get sections bent by them.</t>
+  </si>
+  <si>
+    <t>Not direct companies - but collaboration with CU3D</t>
   </si>
 </sst>
 </file>
@@ -418,9 +473,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
-    <numFmt numFmtId="166" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="6" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="165" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -478,7 +533,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -488,6 +543,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0000FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -505,20 +578,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="6" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1432,18 +1510,18 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.5" customWidth="1"/>
+    <col min="1" max="1" width="30.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1451,7 +1529,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -1459,7 +1537,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1468,7 +1546,7 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1476,7 +1554,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1485,13 +1563,13 @@
       </c>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>64</v>
       </c>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1500,7 +1578,7 @@
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1509,7 +1587,7 @@
       </c>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1518,7 +1596,7 @@
       </c>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1529,16 +1607,16 @@
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c r="B12">
-        <v>2</v>
+      <c r="B12" t="s">
+        <v>120</v>
       </c>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1547,7 +1625,7 @@
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1558,7 +1636,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -1566,7 +1644,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1574,31 +1652,29 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="4">
-        <v>50</v>
-      </c>
-      <c r="C17" s="9">
         <v>500</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C17" s="9"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>50</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="6"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -1606,7 +1682,7 @@
         <v>44850</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -1614,10 +1690,10 @@
         <v>44851</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -1625,29 +1701,29 @@
         <v>44858</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>32</v>
       </c>
       <c r="B24" s="3">
-        <v>44864</v>
+        <v>44875</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>38</v>
       </c>
       <c r="B25" s="3">
-        <v>44867</v>
+        <v>44877</v>
       </c>
       <c r="C25" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1655,15 +1731,18 @@
         <v>44874</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>34</v>
       </c>
       <c r="B27" s="3">
         <v>44888</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -1672,58 +1751,58 @@
       </c>
       <c r="C28" s="6"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34" s="3"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B35" s="3"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B36" s="3"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B37" s="3"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B38" s="3"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B39" s="3"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B41" s="3"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B42" s="3"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B43" s="3"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B44" s="3"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B45" s="3"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B46" s="3"/>
     </row>
   </sheetData>
@@ -1767,7 +1846,40 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="C105" zoomScale="136" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="R166" sqref="R166"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F8467D7-9F6C-4031-9999-C1371BFAAB31}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C45"/>
   <sheetViews>
@@ -1775,18 +1887,18 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1794,7 +1906,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -1802,7 +1914,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1811,15 +1923,15 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1828,7 +1940,7 @@
       </c>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>65</v>
       </c>
@@ -1837,7 +1949,7 @@
       </c>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1846,7 +1958,7 @@
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1855,7 +1967,7 @@
       </c>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1864,7 +1976,7 @@
       </c>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1872,7 +1984,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1881,7 +1993,7 @@
       </c>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1890,7 +2002,7 @@
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1898,7 +2010,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -1906,7 +2018,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1914,7 +2026,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -1923,7 +2035,7 @@
       </c>
       <c r="C17" s="6"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -1932,13 +2044,13 @@
       </c>
       <c r="C18" s="6"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -1946,7 +2058,7 @@
         <v>44858</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -1955,7 +2067,7 @@
       </c>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>71</v>
       </c>
@@ -1963,7 +2075,7 @@
         <v>44872</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -1974,7 +2086,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -1982,7 +2094,7 @@
         <v>44895</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -1990,7 +2102,7 @@
         <v>44949</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -1999,58 +2111,58 @@
       </c>
       <c r="C27" s="6"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B28" s="3"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34" s="3"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B35" s="3"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B36" s="3"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B37" s="3"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B38" s="3"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B39" s="3"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B41" s="3"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B42" s="3"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B43" s="3"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B44" s="3"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B45" s="3"/>
     </row>
   </sheetData>
@@ -2094,26 +2206,26 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68AAC58C-EBDA-3946-A752-4A750B3F87FB}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.5" customWidth="1"/>
+    <col min="1" max="1" width="30.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2121,10 +2233,10 @@
         <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -2132,7 +2244,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2141,7 +2253,7 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2149,7 +2261,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -2158,10 +2270,10 @@
       </c>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -2170,7 +2282,7 @@
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2179,7 +2291,7 @@
       </c>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2188,7 +2300,7 @@
       </c>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -2196,16 +2308,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>20</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -2214,15 +2326,15 @@
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -2230,7 +2342,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -2238,7 +2350,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -2247,7 +2359,7 @@
       </c>
       <c r="C17" s="6"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -2256,109 +2368,120 @@
       </c>
       <c r="C18" s="6"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B21" s="12">
+        <v>44852</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B22" s="3">
         <v>44862</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B23" s="3">
         <v>44864</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>125</v>
-      </c>
-      <c r="B23" s="12">
+      <c r="C23" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" s="12">
         <v>44874</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B25" s="3">
         <v>44880</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B26" s="3">
         <v>44895</v>
       </c>
-      <c r="C25" s="6"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B28" s="3"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C26" s="6"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34" s="3"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B35" s="3"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B36" s="3"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B37" s="3"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B38" s="3"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B39" s="3"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B41" s="3"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B42" s="3"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B43" s="3"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B44" s="3"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B45" s="3"/>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B46" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B6">
@@ -2401,7 +2524,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71F63D42-6AB1-3F4D-96FB-66922EEFB734}">
   <dimension ref="A1:G47"/>
   <sheetViews>
@@ -2409,18 +2532,18 @@
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2428,7 +2551,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -2436,7 +2559,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2445,7 +2568,7 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2453,7 +2576,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -2462,21 +2585,21 @@
       </c>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C8" s="5"/>
       <c r="E8" s="1"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2487,7 +2610,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2498,7 +2621,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -2506,10 +2629,10 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -2517,11 +2640,11 @@
         <v>2</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -2531,7 +2654,7 @@
       <c r="C13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2539,15 +2662,15 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -2555,7 +2678,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -2566,18 +2689,18 @@
       <c r="F17" s="4"/>
       <c r="G17" s="6"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>50</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C18" s="6"/>
       <c r="F18" s="4"/>
       <c r="G18" s="6"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
@@ -2585,7 +2708,7 @@
       <c r="E20" s="1"/>
       <c r="G20" s="5"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -2594,7 +2717,7 @@
       </c>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -2605,7 +2728,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -2614,7 +2737,7 @@
       </c>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -2626,7 +2749,7 @@
       </c>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -2635,7 +2758,7 @@
       </c>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -2644,63 +2767,63 @@
       </c>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C27" s="6"/>
       <c r="F27" s="3"/>
       <c r="G27" s="6"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34" s="3"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B35" s="3"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B36" s="3"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B37" s="3"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B38" s="3"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B39" s="3"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B41" s="3"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B42" s="3"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B43" s="3"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B44" s="3"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B45" s="3"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B46" s="3"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B47" s="3"/>
     </row>
   </sheetData>
@@ -2744,26 +2867,26 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{334B9EB9-B089-5E48-8492-97FB81759DDC}">
   <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2771,7 +2894,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -2779,7 +2902,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2788,7 +2911,7 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2796,7 +2919,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -2805,21 +2928,19 @@
       </c>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2827,10 +2948,10 @@
         <v>44883</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2839,7 +2960,7 @@
       </c>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -2847,7 +2968,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -2856,7 +2977,7 @@
       </c>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -2865,7 +2986,7 @@
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2873,10 +2994,10 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -2884,7 +3005,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -2892,18 +3013,18 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="4">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="C17" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -2912,13 +3033,13 @@
       </c>
       <c r="C18" s="6"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -2926,7 +3047,7 @@
         <v>44859</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -2935,7 +3056,7 @@
       </c>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>83</v>
       </c>
@@ -2943,7 +3064,7 @@
         <v>44875</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -2951,10 +3072,10 @@
         <v>44876</v>
       </c>
       <c r="C24" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -2962,7 +3083,7 @@
         <v>44895</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -2970,7 +3091,7 @@
         <v>44897</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -2979,58 +3100,58 @@
       </c>
       <c r="C27" s="6"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B28" s="3"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34" s="3"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B35" s="3"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B36" s="3"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B37" s="3"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B38" s="3"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B39" s="3"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B41" s="3"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B42" s="3"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B43" s="3"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B44" s="3"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B45" s="3"/>
     </row>
   </sheetData>
@@ -3074,21 +3195,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{121E824B-83DD-034B-8EDA-A3B7621BAB3E}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.33203125" customWidth="1"/>
+    <col min="1" max="1" width="30.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3096,7 +3217,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -3104,7 +3225,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -3112,28 +3233,29 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="16"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -3144,7 +3266,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -3152,7 +3274,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -3163,12 +3285,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C10" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -3179,7 +3301,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -3190,7 +3312,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -3201,7 +3323,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -3209,7 +3331,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -3220,7 +3342,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -3231,7 +3353,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -3239,7 +3361,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -3250,7 +3372,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -3258,7 +3380,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -3269,7 +3391,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -3278,7 +3400,7 @@
       </c>
       <c r="C21" s="6"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
@@ -3286,7 +3408,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -3294,7 +3416,7 @@
         <v>44865</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -3305,7 +3427,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -3313,7 +3435,7 @@
         <v>44884</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -3321,7 +3443,7 @@
         <v>44898</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -3332,7 +3454,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -3340,7 +3462,7 @@
         <v>44954</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -3348,7 +3470,7 @@
         <v>44961</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -3356,7 +3478,7 @@
         <v>44982</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -3367,58 +3489,58 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34" s="3"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B35" s="3"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B36" s="3"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B37" s="3"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B38" s="3"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B39" s="3"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B41" s="3"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B42" s="3"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B43" s="3"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B44" s="3"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B45" s="3"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B46" s="3"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B47" s="3"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B48" s="3"/>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B49" s="3"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B50" s="3"/>
     </row>
   </sheetData>
@@ -3462,157 +3584,212 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BE59ABF-F952-490F-B319-5676379536F1}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A11:G28"/>
   <sheetViews>
     <sheetView zoomScale="159" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C13" t="s">
         <v>95</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="C14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B15" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C15" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D17" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="C5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>107</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C18" s="11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>108</v>
       </c>
-      <c r="C7" s="10" t="s">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>112</v>
+      </c>
+      <c r="C20" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
         <v>109</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E21" t="s">
+        <v>134</v>
+      </c>
+      <c r="F21" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>112</v>
-      </c>
-      <c r="B8" s="10" t="s">
+      <c r="E22" s="13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
         <v>111</v>
       </c>
-      <c r="C8" s="11">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>117</v>
-      </c>
-      <c r="C10" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>116</v>
+      <c r="E23" s="13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>128</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="F24" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>129</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>135</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="F26" t="s">
+        <v>137</v>
+      </c>
+      <c r="G26" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>138</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="F27" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>141</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="F28" t="s">
+        <v>137</v>
+      </c>
+      <c r="G28" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" xr:uid="{2871A78B-D677-4719-A904-680F6B9FAA19}"/>
-    <hyperlink ref="B4" r:id="rId2" display="https://uk.rs-online.com/web/p/hose-connectors/5067294?cm_mmc=UK-PLA-DS3A-_-google-_-CSS_UK_EN_Plumbing_%26_Pipeline_Whoop-_-Hose+Connectors_Whoop+(2)-_-5067294&amp;matchtype=&amp;pla-336450067867&amp;cq_src=google_ads&amp;cq_cmp=9771206590&amp;cq_term=&amp;cq_plac=&amp;cq_net=g&amp;cq_plt=gp&amp;gclsrc=ds&amp;gclsrc=ds" xr:uid="{5230C63F-A465-4067-8459-98FAE5809525}"/>
-    <hyperlink ref="B5" r:id="rId3" display="https://www.ebay.co.uk/itm/124646329429?chn=ps&amp;var=425578763990&amp;_trkparms=ispr%3D1&amp;amdata=enc%3A1Y343ZoYXR9OK7UZzV6tvsA74&amp;norover=1&amp;mkevt=1&amp;mkrid=710-134428-41853-0&amp;mkcid=2&amp;mkscid=101&amp;itemid=425578763990_124646329429&amp;targetid=1647205089320&amp;device=c&amp;mktype=pla&amp;googleloc=1006598&amp;poi=&amp;campaignid=17206177401&amp;mkgroupid=136851690655&amp;rlsatarget=pla-1647205089320&amp;abcId=9300866&amp;merchantid=113804710" xr:uid="{47D68646-9550-4A6B-AEE4-31D267FBF4E5}"/>
-    <hyperlink ref="C7" r:id="rId4" xr:uid="{BFA99E16-C650-4732-B0A3-EA6B38529AF5}"/>
-    <hyperlink ref="B8" r:id="rId5" xr:uid="{3A8E005B-9C46-4615-A032-452300CEC9D3}"/>
+    <hyperlink ref="B11" r:id="rId1" xr:uid="{2871A78B-D677-4719-A904-680F6B9FAA19}"/>
+    <hyperlink ref="B14" r:id="rId2" display="https://uk.rs-online.com/web/p/hose-connectors/5067294?cm_mmc=UK-PLA-DS3A-_-google-_-CSS_UK_EN_Plumbing_%26_Pipeline_Whoop-_-Hose+Connectors_Whoop+(2)-_-5067294&amp;matchtype=&amp;pla-336450067867&amp;cq_src=google_ads&amp;cq_cmp=9771206590&amp;cq_term=&amp;cq_plac=&amp;cq_net=g&amp;cq_plt=gp&amp;gclsrc=ds&amp;gclsrc=ds" xr:uid="{5230C63F-A465-4067-8459-98FAE5809525}"/>
+    <hyperlink ref="B15" r:id="rId3" display="https://www.ebay.co.uk/itm/124646329429?chn=ps&amp;var=425578763990&amp;_trkparms=ispr%3D1&amp;amdata=enc%3A1Y343ZoYXR9OK7UZzV6tvsA74&amp;norover=1&amp;mkevt=1&amp;mkrid=710-134428-41853-0&amp;mkcid=2&amp;mkscid=101&amp;itemid=425578763990_124646329429&amp;targetid=1647205089320&amp;device=c&amp;mktype=pla&amp;googleloc=1006598&amp;poi=&amp;campaignid=17206177401&amp;mkgroupid=136851690655&amp;rlsatarget=pla-1647205089320&amp;abcId=9300866&amp;merchantid=113804710" xr:uid="{47D68646-9550-4A6B-AEE4-31D267FBF4E5}"/>
+    <hyperlink ref="C17" r:id="rId4" xr:uid="{BFA99E16-C650-4732-B0A3-EA6B38529AF5}"/>
+    <hyperlink ref="B18" r:id="rId5" xr:uid="{3A8E005B-9C46-4615-A032-452300CEC9D3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView topLeftCell="C105" zoomScale="136" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="R166" sqref="R166"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated timelines and added ideas and minutes from meeting
</commit_message>
<xml_diff>
--- a/Timelines/powertrain projects.xlsx
+++ b/Timelines/powertrain projects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Retro\OneDrive\Documents\FBR work\Powertrain Repo\Powertrain-Projects-FBR23\Timelines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D1710E-A2D5-453F-886E-5D7F1F4CB02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D192C628-05E6-47DD-9F3B-2B51C436250E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exhaust" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="151">
   <si>
     <t>Task 1:</t>
   </si>
@@ -478,6 +478,15 @@
   </si>
   <si>
     <t>Further details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manufacture of all components for final design </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final version assembly </t>
+  </si>
+  <si>
+    <t>DONE</t>
   </si>
 </sst>
 </file>
@@ -1521,18 +1530,18 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="30.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.453125" customWidth="1"/>
+    <col min="1" max="1" width="30.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1540,7 +1549,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -1548,7 +1557,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1557,7 +1566,7 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1565,7 +1574,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1574,13 +1583,13 @@
       </c>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>64</v>
       </c>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1589,7 +1598,7 @@
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1598,7 +1607,7 @@
       </c>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1607,7 +1616,7 @@
       </c>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1618,7 +1627,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1627,7 +1636,7 @@
       </c>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1636,7 +1645,7 @@
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1647,7 +1656,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -1655,7 +1664,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1663,7 +1672,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -1672,20 +1681,20 @@
       </c>
       <c r="C17" s="9"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>50</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="6"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -1693,7 +1702,7 @@
         <v>44850</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -1704,7 +1713,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -1712,7 +1721,7 @@
         <v>44858</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -1723,7 +1732,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -1734,7 +1743,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1742,7 +1751,7 @@
         <v>44874</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -1753,7 +1762,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -1762,58 +1771,58 @@
       </c>
       <c r="C28" s="6"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B34" s="3"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B35" s="3"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B36" s="3"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B37" s="3"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B38" s="3"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B39" s="3"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B41" s="3"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B42" s="3"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B43" s="3"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B44" s="3"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B45" s="3"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B46" s="3"/>
     </row>
   </sheetData>
@@ -1865,7 +1874,7 @@
       <selection activeCell="R166" sqref="R166"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1878,9 +1887,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>125</v>
       </c>
@@ -1892,24 +1901,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="30.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1917,7 +1926,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -1925,7 +1934,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1934,7 +1943,7 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1942,7 +1951,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1951,7 +1960,7 @@
       </c>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>65</v>
       </c>
@@ -1960,7 +1969,7 @@
       </c>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1969,7 +1978,7 @@
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1978,7 +1987,7 @@
       </c>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1987,7 +1996,7 @@
       </c>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1995,7 +2004,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -2004,7 +2013,7 @@
       </c>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -2013,7 +2022,7 @@
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2021,7 +2030,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -2029,7 +2038,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -2037,7 +2046,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -2046,7 +2055,7 @@
       </c>
       <c r="C17" s="6"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -2055,13 +2064,13 @@
       </c>
       <c r="C18" s="6"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -2069,16 +2078,21 @@
         <v>44858</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>37</v>
       </c>
       <c r="B22" s="3">
         <v>44860</v>
       </c>
-      <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C22" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>71</v>
       </c>
@@ -2086,7 +2100,7 @@
         <v>44872</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -2097,84 +2111,92 @@
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>33</v>
       </c>
       <c r="B25" s="3">
+        <v>44882</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>148</v>
+      </c>
+      <c r="B26" s="3">
         <v>44895</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" s="3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>149</v>
+      </c>
+      <c r="B27" s="3">
         <v>44949</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+      <c r="C27" s="6"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B28" s="3">
         <v>44972</v>
       </c>
-      <c r="C27" s="6"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B28" s="3"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B34" s="3"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B35" s="3"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B36" s="3"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B37" s="3"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B38" s="3"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B39" s="3"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B41" s="3"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B42" s="3"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B43" s="3"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B44" s="3"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B45" s="3"/>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B46" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B6:B7">
@@ -2225,18 +2247,18 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="30.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.453125" customWidth="1"/>
+    <col min="1" max="1" width="30.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2247,7 +2269,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -2255,7 +2277,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2264,7 +2286,7 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2272,7 +2294,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -2281,10 +2303,10 @@
       </c>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -2293,7 +2315,7 @@
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2302,7 +2324,7 @@
       </c>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2311,7 +2333,7 @@
       </c>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -2319,7 +2341,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -2328,7 +2350,7 @@
       </c>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -2337,7 +2359,7 @@
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2345,7 +2367,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -2353,7 +2375,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -2361,7 +2383,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -2370,7 +2392,7 @@
       </c>
       <c r="C17" s="6"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -2379,13 +2401,13 @@
       </c>
       <c r="C18" s="6"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>127</v>
       </c>
@@ -2396,7 +2418,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -2404,7 +2426,7 @@
         <v>44862</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -2415,7 +2437,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>119</v>
       </c>
@@ -2423,7 +2445,7 @@
         <v>44874</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -2431,7 +2453,7 @@
         <v>44880</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -2440,58 +2462,58 @@
       </c>
       <c r="C26" s="6"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B34" s="3"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B35" s="3"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B36" s="3"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B37" s="3"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B38" s="3"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B39" s="3"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B41" s="3"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B42" s="3"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B43" s="3"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B44" s="3"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B45" s="3"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B46" s="3"/>
     </row>
   </sheetData>
@@ -2543,18 +2565,18 @@
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="30.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.46484375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2562,7 +2584,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -2570,7 +2592,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2579,7 +2601,7 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2587,7 +2609,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -2596,10 +2618,10 @@
       </c>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -2610,7 +2632,7 @@
       <c r="E8" s="1"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2621,7 +2643,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2632,7 +2654,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -2643,7 +2665,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -2655,7 +2677,7 @@
       </c>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -2665,7 +2687,7 @@
       <c r="C13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2673,7 +2695,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -2681,7 +2703,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -2689,7 +2711,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -2700,7 +2722,7 @@
       <c r="F17" s="4"/>
       <c r="G17" s="6"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -2711,7 +2733,7 @@
       <c r="F18" s="4"/>
       <c r="G18" s="6"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
@@ -2719,7 +2741,7 @@
       <c r="E20" s="1"/>
       <c r="G20" s="5"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -2728,7 +2750,7 @@
       </c>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -2739,7 +2761,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -2748,7 +2770,7 @@
       </c>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -2760,7 +2782,7 @@
       </c>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -2769,7 +2791,7 @@
       </c>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -2778,63 +2800,63 @@
       </c>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C27" s="6"/>
       <c r="F27" s="3"/>
       <c r="G27" s="6"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B34" s="3"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B35" s="3"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B36" s="3"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B37" s="3"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B38" s="3"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B39" s="3"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B41" s="3"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B42" s="3"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B43" s="3"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B44" s="3"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B45" s="3"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B46" s="3"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B47" s="3"/>
     </row>
   </sheetData>
@@ -2886,18 +2908,18 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="30.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2905,7 +2927,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -2913,7 +2935,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2922,7 +2944,7 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2930,7 +2952,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -2939,10 +2961,10 @@
       </c>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -2951,7 +2973,7 @@
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2962,7 +2984,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2971,7 +2993,7 @@
       </c>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -2979,7 +3001,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -2988,7 +3010,7 @@
       </c>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -2997,7 +3019,7 @@
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -3008,7 +3030,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -3016,7 +3038,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -3024,7 +3046,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -3035,7 +3057,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -3044,13 +3066,13 @@
       </c>
       <c r="C18" s="6"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -3058,7 +3080,7 @@
         <v>44859</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -3067,7 +3089,7 @@
       </c>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>83</v>
       </c>
@@ -3075,7 +3097,7 @@
         <v>44875</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -3086,7 +3108,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -3094,7 +3116,7 @@
         <v>44895</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -3102,7 +3124,7 @@
         <v>44897</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -3111,58 +3133,58 @@
       </c>
       <c r="C27" s="6"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B28" s="3"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B34" s="3"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B35" s="3"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B36" s="3"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B37" s="3"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B38" s="3"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B39" s="3"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B41" s="3"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B42" s="3"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B43" s="3"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B44" s="3"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B45" s="3"/>
     </row>
   </sheetData>
@@ -3214,13 +3236,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="30.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.36328125" customWidth="1"/>
+    <col min="1" max="1" width="30.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3228,7 +3250,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -3236,7 +3258,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -3244,12 +3266,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -3257,7 +3279,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -3266,7 +3288,7 @@
       </c>
       <c r="C6" s="15"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -3277,7 +3299,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -3285,7 +3307,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -3296,12 +3318,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C10" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -3312,7 +3334,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -3323,7 +3345,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -3334,7 +3356,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -3342,7 +3364,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -3353,7 +3375,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -3364,7 +3386,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -3372,7 +3394,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -3383,7 +3405,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -3391,7 +3413,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -3402,7 +3424,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -3411,7 +3433,7 @@
       </c>
       <c r="C21" s="6"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
@@ -3419,7 +3441,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -3427,7 +3449,7 @@
         <v>44865</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -3438,7 +3460,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -3446,7 +3468,7 @@
         <v>44884</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -3454,7 +3476,7 @@
         <v>44898</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -3465,7 +3487,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -3473,7 +3495,7 @@
         <v>44954</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -3481,7 +3503,7 @@
         <v>44961</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -3489,7 +3511,7 @@
         <v>44982</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -3500,58 +3522,58 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B34" s="3"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B35" s="3"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B36" s="3"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B37" s="3"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B38" s="3"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B39" s="3"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B41" s="3"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B42" s="3"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B43" s="3"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B44" s="3"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B45" s="3"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B46" s="3"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B47" s="3"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B48" s="3"/>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B49" s="3"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B50" s="3"/>
     </row>
   </sheetData>
@@ -3601,7 +3623,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3612,13 +3634,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BE59ABF-F952-490F-B319-5676379536F1}">
   <dimension ref="A7:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="159" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="159" workbookViewId="0">
       <selection activeCell="F21" sqref="B21:F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>144</v>
       </c>
@@ -3632,7 +3654,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>89</v>
       </c>
@@ -3643,7 +3665,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>92</v>
       </c>
@@ -3651,7 +3673,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>94</v>
       </c>
@@ -3659,7 +3681,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>100</v>
       </c>
@@ -3670,7 +3692,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B15" s="10" t="s">
         <v>97</v>
       </c>
@@ -3678,12 +3700,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>102</v>
       </c>
@@ -3697,7 +3719,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>107</v>
       </c>
@@ -3708,12 +3730,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>112</v>
       </c>
@@ -3721,7 +3743,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B21" s="1" t="s">
         <v>109</v>
       </c>
@@ -3734,7 +3756,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
         <v>110</v>
       </c>
@@ -3742,7 +3764,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
         <v>111</v>
       </c>
@@ -3750,7 +3772,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
         <v>128</v>
       </c>
@@ -3761,7 +3783,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
         <v>129</v>
       </c>
@@ -3769,7 +3791,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
         <v>135</v>
       </c>
@@ -3783,7 +3805,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B27" t="s">
         <v>138</v>
       </c>
@@ -3794,7 +3816,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
         <v>141</v>
       </c>

</xml_diff>

<commit_message>
Updated timelines - mid November, come projects delayed with exhaust project at severe risk of delay
</commit_message>
<xml_diff>
--- a/Timelines/powertrain projects.xlsx
+++ b/Timelines/powertrain projects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Retro\OneDrive\Documents\FBR work\Powertrain Repo\Powertrain-Projects-FBR23\Timelines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D192C628-05E6-47DD-9F3B-2B51C436250E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6355017A-F36E-4ABC-934A-93132BA42986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exhaust" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="154">
   <si>
     <t>Task 1:</t>
   </si>
@@ -258,9 +258,6 @@
     <t>Aidan &amp; Joel</t>
   </si>
   <si>
-    <t>3D printing</t>
-  </si>
-  <si>
     <t>attention to prevent repeat of fbr22 intake incident. not very prototypable, pay attention to not throw money &amp; time out the window</t>
   </si>
   <si>
@@ -300,9 +297,6 @@
     <t>1 fresher prototype</t>
   </si>
   <si>
-    <t>?TD</t>
-  </si>
-  <si>
     <t>Fuel Injectors</t>
   </si>
   <si>
@@ -414,9 +408,6 @@
     <t>Estimation of timeline for Gear position sensor from Arnav - based on plausibility</t>
   </si>
   <si>
-    <t>TD - meeting slot for Diff hangers</t>
-  </si>
-  <si>
     <t>Design discussions</t>
   </si>
   <si>
@@ -435,9 +426,6 @@
     <t>Can or fluids iterations can trickle into Xmas</t>
   </si>
   <si>
-    <t>CURRENT UPDATE REQUIRED</t>
-  </si>
-  <si>
     <t>Contacted</t>
   </si>
   <si>
@@ -487,6 +475,27 @@
   </si>
   <si>
     <t>DONE</t>
+  </si>
+  <si>
+    <t>TD - done</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TD </t>
+  </si>
+  <si>
+    <t>3D printing - collaboration and further involvement from 3D print soc, they can provide filament which saves significant proportion of the costs</t>
+  </si>
+  <si>
+    <t>DELAYED</t>
+  </si>
+  <si>
+    <t>PROJECT COMPLETED</t>
+  </si>
+  <si>
+    <t>SEVERELY DELAYED - AT RISK OF IMPEDING DYNO DATE</t>
   </si>
 </sst>
 </file>
@@ -554,7 +563,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -585,6 +594,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -599,7 +614,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -614,9 +629,10 @@
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -647,6 +663,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFCC00CC"/>
         </patternFill>
       </fill>
@@ -767,27 +804,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1526,8 +1542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8AD9B51-42AD-FC45-A027-363DE91F3909}">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1554,7 +1570,7 @@
         <v>44</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>45</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
@@ -1624,7 +1640,7 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
@@ -1632,7 +1648,7 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C12" s="5"/>
     </row>
@@ -1710,7 +1726,7 @@
         <v>44851</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
@@ -1729,7 +1745,7 @@
         <v>44875</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
@@ -1740,7 +1756,7 @@
         <v>44877</v>
       </c>
       <c r="C25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
@@ -1759,7 +1775,7 @@
         <v>44888</v>
       </c>
       <c r="C27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
@@ -1885,13 +1901,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F8467D7-9F6C-4031-9999-C1371BFAAB31}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1903,8 +1921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1948,7 +1966,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
@@ -2043,7 +2061,7 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>74</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
@@ -2060,7 +2078,7 @@
         <v>50</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C18" s="6"/>
     </row>
@@ -2086,10 +2104,10 @@
         <v>44860</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D22" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
@@ -2108,7 +2126,10 @@
         <v>44876</v>
       </c>
       <c r="C24" t="s">
-        <v>84</v>
+        <v>149</v>
+      </c>
+      <c r="D24" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
@@ -2121,7 +2142,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B26" s="3">
         <v>44895</v>
@@ -2129,7 +2150,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B27" s="3">
         <v>44949</v>
@@ -2241,10 +2262,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68AAC58C-EBDA-3946-A752-4A750B3F87FB}">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2253,12 +2274,12 @@
     <col min="2" max="2" width="45.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2266,18 +2287,18 @@
         <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B3" s="16" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2285,8 +2306,9 @@
         <v>2</v>
       </c>
       <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E4" s="14"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2294,7 +2316,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -2303,10 +2325,10 @@
       </c>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -2315,7 +2337,7 @@
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2324,7 +2346,7 @@
       </c>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2333,7 +2355,7 @@
       </c>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -2341,7 +2363,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -2350,24 +2372,24 @@
       </c>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -2375,7 +2397,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -2409,13 +2431,13 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B21" s="12">
         <v>44852</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
@@ -2434,12 +2456,12 @@
         <v>44864</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B24" s="12">
         <v>44874</v>
@@ -2542,13 +2564,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="containsText" dxfId="23" priority="1" operator="containsText" text="cancelled">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="cancelled">
       <formula>NOT(ISERROR(SEARCH("cancelled",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="2" operator="containsText" text="delayed">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="delayed">
       <formula>NOT(ISERROR(SEARCH("delayed",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="3" operator="containsText" text="on time">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="on time">
       <formula>NOT(ISERROR(SEARCH("on time",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2626,7 +2648,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C8" s="5"/>
       <c r="E8" s="1"/>
@@ -2662,7 +2684,7 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
@@ -2673,7 +2695,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G12" s="5"/>
     </row>
@@ -2682,7 +2704,7 @@
         <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C13" s="1"/>
       <c r="G13" s="1"/>
@@ -2692,7 +2714,7 @@
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
@@ -2700,7 +2722,7 @@
         <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
@@ -2727,7 +2749,7 @@
         <v>50</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C18" s="6"/>
       <c r="F18" s="4"/>
@@ -2778,7 +2800,7 @@
         <v>44918</v>
       </c>
       <c r="C24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F24" s="3"/>
     </row>
@@ -2861,16 +2883,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B6">
-    <cfRule type="cellIs" dxfId="20" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="5" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="6" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="7" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2885,13 +2907,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="containsText" dxfId="16" priority="1" operator="containsText" text="cancelled">
+    <cfRule type="containsText" dxfId="19" priority="1" operator="containsText" text="cancelled">
       <formula>NOT(ISERROR(SEARCH("cancelled",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="2" operator="containsText" text="delayed">
+    <cfRule type="containsText" dxfId="18" priority="2" operator="containsText" text="delayed">
       <formula>NOT(ISERROR(SEARCH("delayed",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="3" operator="containsText" text="on time">
+    <cfRule type="containsText" dxfId="17" priority="3" operator="containsText" text="on time">
       <formula>NOT(ISERROR(SEARCH("on time",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2905,7 +2927,7 @@
   <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2924,7 +2946,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -2949,7 +2971,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
@@ -2981,7 +3003,7 @@
         <v>44883</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
@@ -3027,7 +3049,7 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
@@ -3035,7 +3057,7 @@
         <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
@@ -3043,7 +3065,7 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
@@ -3054,7 +3076,7 @@
         <v>100</v>
       </c>
       <c r="C17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
@@ -3062,7 +3084,7 @@
         <v>50</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C18" s="6"/>
     </row>
@@ -3091,7 +3113,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B23" s="3">
         <v>44875</v>
@@ -3105,7 +3127,7 @@
         <v>44876</v>
       </c>
       <c r="C24" t="s">
-        <v>88</v>
+        <v>148</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
@@ -3189,16 +3211,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B6">
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3213,13 +3235,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="cancelled">
+    <cfRule type="containsText" dxfId="12" priority="1" operator="containsText" text="cancelled">
       <formula>NOT(ISERROR(SEARCH("cancelled",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="delayed">
+    <cfRule type="containsText" dxfId="11" priority="2" operator="containsText" text="delayed">
       <formula>NOT(ISERROR(SEARCH("delayed",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="on time">
+    <cfRule type="containsText" dxfId="10" priority="3" operator="containsText" text="on time">
       <formula>NOT(ISERROR(SEARCH("on time",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3233,7 +3255,7 @@
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3276,17 +3298,17 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="C6" s="15"/>
+      <c r="B6" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" s="14"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
@@ -3578,16 +3600,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3602,13 +3624,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="cancelled">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="cancelled">
       <formula>NOT(ISERROR(SEARCH("cancelled",B6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="delayed">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="delayed">
       <formula>NOT(ISERROR(SEARCH("delayed",B6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="on time">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="on time">
       <formula>NOT(ISERROR(SEARCH("on time",B6)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3634,7 +3656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BE59ABF-F952-490F-B319-5676379536F1}">
   <dimension ref="A7:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="159" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="159" workbookViewId="0">
       <selection activeCell="F21" sqref="B21:F21"/>
     </sheetView>
   </sheetViews>
@@ -3642,89 +3664,89 @@
   <sheetData>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B7" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C7" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E7" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" t="s">
         <v>89</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C11" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B15" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
+        <v>100</v>
+      </c>
+      <c r="B17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="B17" t="s">
+      <c r="D17" t="s">
         <v>103</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="D17" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C18" s="11">
         <v>30</v>
@@ -3732,102 +3754,102 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B21" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F24" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F26" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G26" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B27" t="s">
-        <v>138</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>139</v>
+        <v>134</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>135</v>
       </c>
       <c r="F27" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
-        <v>141</v>
-      </c>
-      <c r="E28" s="16" t="s">
-        <v>139</v>
+        <v>137</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>135</v>
       </c>
       <c r="F28" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G28" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>